<commit_message>
update code & output
</commit_message>
<xml_diff>
--- a/stata_gen_yaml/Documentation/unit_harmonization.xlsx
+++ b/stata_gen_yaml/Documentation/unit_harmonization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smccutchan\OneDrive - Research Triangle Institute\Documents\DMC\YAMLTransforms\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68DF0973-B710-4600-92BE-AD55626041A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065EC3D7-F5C3-48C9-BA33-73576285269B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{0BF9606B-C022-481E-9D8C-ECB683C8FC4F}"/>
+    <workbookView xWindow="0" yWindow="10880" windowWidth="19200" windowHeight="11200" activeTab="1" xr2:uid="{0BF9606B-C022-481E-9D8C-ECB683C8FC4F}"/>
   </bookViews>
   <sheets>
     <sheet name="unit_key" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="350">
   <si>
     <t>%</t>
   </si>
@@ -851,9 +851,6 @@
     <t>/ 4</t>
   </si>
   <si>
-    <t>stata_unit</t>
-  </si>
-  <si>
     <t>%{normal}</t>
   </si>
   <si>
@@ -1089,6 +1086,9 @@
   </si>
   <si>
     <t>mL/s</t>
+  </si>
+  <si>
+    <t>dm</t>
   </si>
 </sst>
 </file>
@@ -1104,15 +1104,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1484,19 +1486,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16EAD5BE-E410-43E4-8557-DE7DA492A13C}">
   <dimension ref="A1:C234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="B148" sqref="B148"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.1796875" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
     <col min="3" max="3" width="45" customWidth="1"/>
-    <col min="4" max="4" width="32.1796875" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>149</v>
       </c>
@@ -1507,15 +1509,15 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1523,471 +1525,471 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="B5" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B6" s="4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>188</v>
       </c>
       <c r="B7" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>189</v>
       </c>
       <c r="B8" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>131</v>
       </c>
       <c r="B10" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>134</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B11" s="4" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>89</v>
       </c>
       <c r="B12" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>90</v>
       </c>
       <c r="B13" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>91</v>
       </c>
       <c r="B14" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>124</v>
       </c>
       <c r="B15" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>133</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="4" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>200</v>
       </c>
       <c r="B22" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>135</v>
       </c>
       <c r="B23" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>245</v>
       </c>
       <c r="B24" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>115</v>
       </c>
       <c r="B25" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>70</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B28" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>128</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B29" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>66</v>
       </c>
       <c r="B31" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>127</v>
       </c>
       <c r="B32" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>165</v>
       </c>
       <c r="B33" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>139</v>
       </c>
       <c r="B34" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>114</v>
       </c>
       <c r="B35" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>138</v>
       </c>
       <c r="B36" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>110</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>175</v>
       </c>
       <c r="B38" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>236</v>
       </c>
       <c r="B39" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>176</v>
       </c>
       <c r="B40" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>177</v>
       </c>
       <c r="B41" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>74</v>
       </c>
       <c r="B42" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>249</v>
       </c>
       <c r="B46" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>250</v>
       </c>
       <c r="B47" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>178</v>
       </c>
       <c r="B48" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>76</v>
       </c>
       <c r="B49" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>179</v>
       </c>
       <c r="B50" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>156</v>
       </c>
       <c r="B51" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>237</v>
       </c>
       <c r="B52" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>38</v>
       </c>
       <c r="B54" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>64</v>
       </c>
       <c r="B55" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B56" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>235</v>
       </c>
       <c r="B57" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>141</v>
       </c>
       <c r="B58" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>248</v>
       </c>
       <c r="B59" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>117</v>
       </c>
       <c r="B60" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>39</v>
       </c>
       <c r="B61" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>45</v>
       </c>
@@ -1995,7 +1997,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>46</v>
       </c>
@@ -2003,7 +2005,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>47</v>
       </c>
@@ -2011,7 +2013,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>48</v>
       </c>
@@ -2019,7 +2021,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>49</v>
       </c>
@@ -2027,7 +2029,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>57</v>
       </c>
@@ -2035,7 +2037,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>59</v>
       </c>
@@ -2043,7 +2045,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>60</v>
       </c>
@@ -2051,7 +2053,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>51</v>
       </c>
@@ -2059,175 +2061,175 @@
         <v>51</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71" s="5" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="B71" s="5" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B71" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>172</v>
       </c>
       <c r="B72" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>253</v>
       </c>
       <c r="B73" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>257</v>
       </c>
       <c r="B74" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>53</v>
       </c>
       <c r="B75" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>174</v>
       </c>
       <c r="B76" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>172</v>
       </c>
       <c r="B77" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>119</v>
       </c>
       <c r="B78" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>120</v>
       </c>
       <c r="B79" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>121</v>
       </c>
       <c r="B80" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>232</v>
       </c>
       <c r="B81" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>42</v>
       </c>
       <c r="B82" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>258</v>
       </c>
-      <c r="B83" s="5" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B83" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>173</v>
       </c>
       <c r="B84" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>201</v>
       </c>
       <c r="B85" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>186</v>
       </c>
-      <c r="B86" s="5" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B86" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>184</v>
       </c>
       <c r="B87" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>23</v>
       </c>
       <c r="B88" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>233</v>
       </c>
       <c r="B89" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>247</v>
       </c>
-      <c r="B90" s="5" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B90" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>185</v>
       </c>
       <c r="B91" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>71</v>
       </c>
@@ -2235,39 +2237,39 @@
         <v>70</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>112</v>
       </c>
       <c r="B93" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>228</v>
       </c>
       <c r="B94" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>126</v>
       </c>
       <c r="B95" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>229</v>
       </c>
       <c r="B96" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>136</v>
       </c>
@@ -2275,15 +2277,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>5</v>
       </c>
       <c r="B98" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>75</v>
       </c>
@@ -2291,7 +2293,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>7</v>
       </c>
@@ -2299,15 +2301,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>132</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B101" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>84</v>
       </c>
@@ -2315,7 +2317,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>85</v>
       </c>
@@ -2323,7 +2325,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>86</v>
       </c>
@@ -2331,7 +2333,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>87</v>
       </c>
@@ -2339,85 +2341,85 @@
         <v>132</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>77</v>
       </c>
       <c r="B106" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>78</v>
       </c>
       <c r="B107" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C107" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>111</v>
       </c>
       <c r="B108" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C108" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>79</v>
       </c>
       <c r="B109" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>129</v>
       </c>
-      <c r="B110" s="5" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B110" s="4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>80</v>
       </c>
       <c r="B111" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>130</v>
       </c>
-      <c r="B112" s="5" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B112" s="4" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>81</v>
       </c>
       <c r="B113" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B114" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>196</v>
       </c>
@@ -2425,7 +2427,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>195</v>
       </c>
@@ -2433,7 +2435,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>238</v>
       </c>
@@ -2441,7 +2443,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>82</v>
       </c>
@@ -2449,7 +2451,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>239</v>
       </c>
@@ -2457,55 +2459,55 @@
         <v>82</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>9</v>
       </c>
       <c r="B120" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>194</v>
       </c>
       <c r="B121" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>197</v>
       </c>
       <c r="B122" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>11</v>
       </c>
       <c r="B123" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>219</v>
       </c>
       <c r="B124" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B125" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>15</v>
       </c>
@@ -2513,7 +2515,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>16</v>
       </c>
@@ -2521,106 +2523,106 @@
         <v>16</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>17</v>
       </c>
       <c r="B128" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>92</v>
       </c>
       <c r="B129" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>93</v>
       </c>
       <c r="B130" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>263</v>
       </c>
       <c r="B131" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>251</v>
       </c>
       <c r="B132" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>262</v>
       </c>
       <c r="B133" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>264</v>
       </c>
       <c r="B134" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>109</v>
       </c>
       <c r="B135" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>94</v>
       </c>
       <c r="B136" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>95</v>
       </c>
       <c r="B137" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>240</v>
       </c>
       <c r="B138" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>96</v>
       </c>
       <c r="B139" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C139" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>97</v>
       </c>
@@ -2628,7 +2630,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>99</v>
       </c>
@@ -2636,7 +2638,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>206</v>
       </c>
@@ -2644,7 +2646,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>100</v>
       </c>
@@ -2652,7 +2654,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>18</v>
       </c>
@@ -2660,39 +2662,39 @@
         <v>100</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>98</v>
       </c>
       <c r="B145" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>19</v>
       </c>
       <c r="B146" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>101</v>
       </c>
       <c r="B147" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>211</v>
       </c>
       <c r="B148" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>20</v>
       </c>
@@ -2700,7 +2702,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>207</v>
       </c>
@@ -2708,39 +2710,39 @@
         <v>20</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>21</v>
       </c>
       <c r="B151" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B152" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>22</v>
       </c>
       <c r="B153" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>209</v>
       </c>
       <c r="B154" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>218</v>
       </c>
@@ -2748,7 +2750,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>217</v>
       </c>
@@ -2756,63 +2758,63 @@
         <v>218</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>222</v>
       </c>
       <c r="B157" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>223</v>
       </c>
       <c r="B158" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>224</v>
       </c>
       <c r="B159" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>225</v>
       </c>
       <c r="B160" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B161" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>226</v>
       </c>
       <c r="B162" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
+        <v>347</v>
+      </c>
+      <c r="B163" t="s">
         <v>348</v>
       </c>
-      <c r="B163" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>25</v>
       </c>
@@ -2820,55 +2822,55 @@
         <v>25</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>26</v>
       </c>
       <c r="B165" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>83</v>
       </c>
       <c r="B166" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>227</v>
       </c>
       <c r="B167" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>27</v>
       </c>
       <c r="B168" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>122</v>
       </c>
       <c r="B169" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>123</v>
       </c>
       <c r="B170" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>103</v>
       </c>
@@ -2876,93 +2878,93 @@
         <v>103</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>104</v>
       </c>
       <c r="B172" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C172" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>105</v>
       </c>
       <c r="B173" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C173" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>160</v>
       </c>
       <c r="B174" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>137</v>
       </c>
       <c r="B175" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>106</v>
       </c>
       <c r="B176" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>28</v>
       </c>
       <c r="B177" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>241</v>
       </c>
       <c r="B178" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A179" t="s">
-        <v>311</v>
-      </c>
       <c r="B179" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>242</v>
       </c>
       <c r="B180" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>107</v>
       </c>
       <c r="B181" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>216</v>
       </c>
@@ -2970,7 +2972,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>102</v>
       </c>
@@ -2978,7 +2980,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>29</v>
       </c>
@@ -2986,7 +2988,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>108</v>
       </c>
@@ -2994,47 +2996,47 @@
         <v>29</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>267</v>
       </c>
       <c r="B186" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>30</v>
       </c>
       <c r="B187" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>252</v>
       </c>
       <c r="B188" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A189" t="s">
-        <v>316</v>
-      </c>
       <c r="B189" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>31</v>
       </c>
       <c r="B190" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>2</v>
       </c>
@@ -3042,7 +3044,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>182</v>
       </c>
@@ -3050,7 +3052,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>246</v>
       </c>
@@ -3058,7 +3060,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>243</v>
       </c>
@@ -3066,7 +3068,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>244</v>
       </c>
@@ -3074,7 +3076,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>230</v>
       </c>
@@ -3082,7 +3084,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>231</v>
       </c>
@@ -3090,7 +3092,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>113</v>
       </c>
@@ -3098,31 +3100,31 @@
         <v>113</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>34</v>
       </c>
       <c r="B199" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>35</v>
       </c>
       <c r="B200" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>37</v>
       </c>
       <c r="B201" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>116</v>
       </c>
@@ -3130,63 +3132,63 @@
         <v>140</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>213</v>
       </c>
       <c r="B203" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>145</v>
       </c>
       <c r="B204" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>256</v>
       </c>
       <c r="B205" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>254</v>
       </c>
       <c r="B206" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>202</v>
       </c>
       <c r="B207" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>203</v>
       </c>
       <c r="B208" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>255</v>
       </c>
       <c r="B209" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>212</v>
       </c>
@@ -3194,7 +3196,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>41</v>
       </c>
@@ -3202,7 +3204,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>125</v>
       </c>
@@ -3210,118 +3212,121 @@
         <v>41</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>214</v>
       </c>
       <c r="B213" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>215</v>
       </c>
       <c r="B214" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.35">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B231" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.35">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.35">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>118</v>
       </c>
@@ -3338,765 +3343,456 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A24AC2A4-71DA-4168-88D2-3E864734E945}">
-  <dimension ref="A1:B98"/>
+  <dimension ref="A1:A87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B98" sqref="A2:B98"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.26953125" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>270</v>
       </c>
-      <c r="B1" s="4" t="s">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="5" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="B5" s="5" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="5" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>258</v>
-      </c>
-      <c r="B7" s="5" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>186</v>
-      </c>
-      <c r="B8" s="5" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>247</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="5" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="5" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>132</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>129</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>130</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="5"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>189</v>
-      </c>
-      <c r="B27" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>196</v>
-      </c>
-      <c r="B28" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>239</v>
-      </c>
-      <c r="B29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>219</v>
-      </c>
-      <c r="B31" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>131</v>
-      </c>
-      <c r="B32" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>134</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>133</v>
-      </c>
-      <c r="B34" s="5" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>250</v>
-      </c>
-      <c r="B38" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>15</v>
-      </c>
-      <c r="B39" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>16</v>
-      </c>
-      <c r="B40" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>17</v>
-      </c>
-      <c r="B41" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>135</v>
-      </c>
-      <c r="B42" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>94</v>
-      </c>
-      <c r="B43" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>97</v>
-      </c>
-      <c r="B45" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>100</v>
-      </c>
-      <c r="B46" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>18</v>
-      </c>
-      <c r="B47" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>19</v>
-      </c>
-      <c r="B48" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>20</v>
-      </c>
-      <c r="B49" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>21</v>
-      </c>
-      <c r="B50" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>22</v>
-      </c>
-      <c r="B51" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>209</v>
-      </c>
-      <c r="B52" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>218</v>
-      </c>
-      <c r="B53" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>264</v>
-      </c>
-      <c r="B54" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>263</v>
-      </c>
-      <c r="B55" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>222</v>
-      </c>
-      <c r="B56" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>224</v>
-      </c>
-      <c r="B57" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>24</v>
-      </c>
-      <c r="B58" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>25</v>
-      </c>
-      <c r="B59" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>26</v>
-      </c>
-      <c r="B60" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>103</v>
-      </c>
-      <c r="B61" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>27</v>
-      </c>
-      <c r="B63" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>137</v>
-      </c>
-      <c r="B64" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>28</v>
-      </c>
-      <c r="B65" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>311</v>
-      </c>
-      <c r="B66" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>242</v>
-      </c>
-      <c r="B67" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>29</v>
-      </c>
-      <c r="B68" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>251</v>
-      </c>
-      <c r="B69" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>267</v>
-      </c>
-      <c r="B70" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>30</v>
-      </c>
-      <c r="B71" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>316</v>
       </c>
-      <c r="B72" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>31</v>
-      </c>
-      <c r="B73" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>165</v>
-      </c>
-      <c r="B74" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>139</v>
-      </c>
-      <c r="B75" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>138</v>
-      </c>
-      <c r="B76" t="s">
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>128</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>113</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>34</v>
-      </c>
-      <c r="B79" s="5" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>35</v>
-      </c>
-      <c r="B80" s="5" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>36</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>37</v>
-      </c>
-      <c r="B82" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>38</v>
-      </c>
-      <c r="B83" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>116</v>
-      </c>
-      <c r="B85" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>235</v>
-      </c>
-      <c r="B86" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>141</v>
-      </c>
-      <c r="B87" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
-        <v>117</v>
-      </c>
-      <c r="B88" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
-        <v>127</v>
-      </c>
-      <c r="B91" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
-        <v>254</v>
-      </c>
-      <c r="B92" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
-        <v>203</v>
-      </c>
-      <c r="B93" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
-        <v>255</v>
-      </c>
-      <c r="B94" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
-        <v>145</v>
-      </c>
-      <c r="B95" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
-        <v>41</v>
-      </c>
-      <c r="B96" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
-        <v>215</v>
-      </c>
-      <c r="B97" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
-        <v>126</v>
-      </c>
-      <c r="B98" t="s">
-        <v>334</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A226">
+    <sortCondition ref="A2:A226"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4105,20 +3801,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E288323-9CD1-4B1C-8D0F-8B916B72D5FD}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.453125" customWidth="1"/>
-    <col min="2" max="2" width="15.7265625" customWidth="1"/>
-    <col min="3" max="3" width="20.453125" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="22.453125" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>150</v>
       </c>
@@ -4132,9 +3828,9 @@
         <v>192</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -4143,64 +3839,64 @@
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>283</v>
+      <c r="B3" s="4" t="s">
+        <v>282</v>
       </c>
       <c r="C3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>283</v>
+      <c r="B4" s="4" t="s">
+        <v>282</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>278</v>
+      <c r="B5" s="4" t="s">
+        <v>277</v>
       </c>
       <c r="C5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>292</v>
+      <c r="B7" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="C7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>180</v>
+        <v>349</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -4209,7 +3905,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>132</v>
       </c>
@@ -4220,53 +3916,53 @@
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>285</v>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>284</v>
       </c>
       <c r="B10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B11" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>289</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>285</v>
+        <v>288</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>284</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>289</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>321</v>
+        <v>288</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>320</v>
       </c>
       <c r="D13" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B14" t="s">
         <v>218</v>
@@ -4275,9 +3971,9 @@
         <v>221</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
-        <v>292</v>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -4286,53 +3982,53 @@
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B16" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B19" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B20" t="s">
         <v>15</v>
@@ -4341,128 +4037,128 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>298</v>
+      </c>
+      <c r="B21" t="s">
         <v>299</v>
-      </c>
-      <c r="B21" t="s">
-        <v>300</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B22" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D22" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>299</v>
+      </c>
+      <c r="B23" t="s">
         <v>300</v>
-      </c>
-      <c r="B23" t="s">
-        <v>301</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B24" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C25" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B27" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B28" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>218</v>
       </c>
       <c r="B29" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C29" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B30" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C30" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B31" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>25</v>
       </c>
@@ -4473,177 +4169,177 @@
         <v>181</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>309</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>310</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B34" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B36" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>313</v>
+      </c>
+      <c r="B37" t="s">
         <v>314</v>
-      </c>
-      <c r="B37" t="s">
-        <v>315</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B38" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B39" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>321</v>
+      </c>
+      <c r="B40" t="s">
         <v>322</v>
-      </c>
-      <c r="B40" t="s">
-        <v>323</v>
       </c>
       <c r="D40" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B41" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B42" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>324</v>
+      </c>
+      <c r="B43" t="s">
         <v>325</v>
-      </c>
-      <c r="B43" t="s">
-        <v>326</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B44" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B45" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B46" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B47" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B48" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>146</v>
@@ -4666,15 +4362,15 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" customWidth="1"/>
-    <col min="2" max="3" width="12.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="24.54296875" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>150</v>
       </c>
@@ -4694,12 +4390,12 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -4714,42 +4410,42 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B6" t="s">
         <v>41</v>
@@ -4758,42 +4454,42 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>273</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>274</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>273</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>272</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>103</v>
       </c>
       <c r="B9" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B10" t="s">
         <v>103</v>
@@ -4802,100 +4498,100 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>277</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>274</v>
+        <v>276</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>273</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
-        <v>274</v>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>273</v>
       </c>
       <c r="B12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B14" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>274</v>
+      </c>
+      <c r="B15" t="s">
         <v>275</v>
-      </c>
-      <c r="B15" t="s">
-        <v>276</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B18" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>296</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>274</v>
+        <v>295</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>273</v>
       </c>
       <c r="C19">
         <v>1</v>

</xml_diff>